<commit_message>
fix: Remove IAF-only products from general database
Removed 5 Siège/Densihair products (87557, 87558, 87559, 87560, 87950)
from estoqueplanilha.xlsx as they are IAF products only.

These products remain in iaf_cabelos for IAF analysis.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/estoqueplanilha.xlsx
+++ b/data/estoqueplanilha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15066" uniqueCount="10029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15051" uniqueCount="10019">
   <si>
     <t>SKU</t>
   </si>
@@ -29914,43 +29914,13 @@
     <t>SACHET SIÀGE CAUTERIZAÇÃO DOS LISOS SH/M/COND 3X7ML VENDA</t>
   </si>
   <si>
-    <t>87557</t>
-  </si>
-  <si>
-    <t>Shampoo Siège Volume Imediato 250ml</t>
+    <t>87918</t>
+  </si>
+  <si>
+    <t>LILY COND ACET V2 250ml</t>
   </si>
   <si>
     <t>oBoticário</t>
-  </si>
-  <si>
-    <t>87559</t>
-  </si>
-  <si>
-    <t>Máscara Capilar Siège Volume Imediato 250g</t>
-  </si>
-  <si>
-    <t>87950</t>
-  </si>
-  <si>
-    <t>Sérum Capilar Siège Volume Imediato 100ml</t>
-  </si>
-  <si>
-    <t>87558</t>
-  </si>
-  <si>
-    <t>Condicionador Siège Volume Imediato 200ml</t>
-  </si>
-  <si>
-    <t>87560</t>
-  </si>
-  <si>
-    <t>Mousse Capilar Siège Volume Imediato 150ml</t>
-  </si>
-  <si>
-    <t>87918</t>
-  </si>
-  <si>
-    <t>LILY COND ACET V2 250ml</t>
   </si>
   <si>
     <t>88665</t>
@@ -30153,8 +30123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5023" totalsRowShown="0">
-  <autoFilter ref="A1:C5023"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5018" totalsRowShown="0">
+  <autoFilter ref="A1:C5018"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SKU" dataDxfId="0"/>
     <tableColumn id="2" name="Nome" dataDxfId="0"/>
@@ -30449,7 +30419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5023"/>
+  <dimension ref="A1:C5018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -85479,62 +85449,62 @@
         <v>9986</v>
       </c>
       <c r="C5003" s="1" t="s">
-        <v>9968</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5004" spans="1:3">
       <c r="A5004" s="1" t="s">
+        <v>9988</v>
+      </c>
+      <c r="B5004" s="1" t="s">
+        <v>9989</v>
+      </c>
+      <c r="C5004" s="1" t="s">
         <v>9987</v>
-      </c>
-      <c r="B5004" s="1" t="s">
-        <v>9988</v>
-      </c>
-      <c r="C5004" s="1" t="s">
-        <v>9968</v>
       </c>
     </row>
     <row r="5005" spans="1:3">
       <c r="A5005" s="1" t="s">
-        <v>9989</v>
+        <v>9990</v>
       </c>
       <c r="B5005" s="1" t="s">
-        <v>9990</v>
+        <v>9991</v>
       </c>
       <c r="C5005" s="1" t="s">
-        <v>9968</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5006" spans="1:3">
       <c r="A5006" s="1" t="s">
-        <v>9991</v>
+        <v>9992</v>
       </c>
       <c r="B5006" s="1" t="s">
-        <v>9992</v>
+        <v>9993</v>
       </c>
       <c r="C5006" s="1" t="s">
-        <v>9968</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5007" spans="1:3">
       <c r="A5007" s="1" t="s">
-        <v>9993</v>
+        <v>9994</v>
       </c>
       <c r="B5007" s="1" t="s">
-        <v>9994</v>
+        <v>9995</v>
       </c>
       <c r="C5007" s="1" t="s">
-        <v>9968</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5008" spans="1:3">
       <c r="A5008" s="1" t="s">
-        <v>9995</v>
+        <v>9996</v>
       </c>
       <c r="B5008" s="1" t="s">
-        <v>9996</v>
+        <v>9997</v>
       </c>
       <c r="C5008" s="1" t="s">
-        <v>9997</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5009" spans="1:3">
@@ -85545,7 +85515,7 @@
         <v>9999</v>
       </c>
       <c r="C5009" s="1" t="s">
-        <v>9997</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5010" spans="1:3">
@@ -85556,7 +85526,7 @@
         <v>10001</v>
       </c>
       <c r="C5010" s="1" t="s">
-        <v>9997</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5011" spans="1:3">
@@ -85567,7 +85537,7 @@
         <v>10003</v>
       </c>
       <c r="C5011" s="1" t="s">
-        <v>9997</v>
+        <v>9987</v>
       </c>
     </row>
     <row r="5012" spans="1:3">
@@ -85578,62 +85548,62 @@
         <v>10005</v>
       </c>
       <c r="C5012" s="1" t="s">
-        <v>9997</v>
+        <v>10006</v>
       </c>
     </row>
     <row r="5013" spans="1:3">
       <c r="A5013" s="1" t="s">
+        <v>10007</v>
+      </c>
+      <c r="B5013" s="1" t="s">
+        <v>10008</v>
+      </c>
+      <c r="C5013" s="1" t="s">
         <v>10006</v>
-      </c>
-      <c r="B5013" s="1" t="s">
-        <v>10007</v>
-      </c>
-      <c r="C5013" s="1" t="s">
-        <v>9997</v>
       </c>
     </row>
     <row r="5014" spans="1:3">
       <c r="A5014" s="1" t="s">
-        <v>10008</v>
+        <v>10009</v>
       </c>
       <c r="B5014" s="1" t="s">
-        <v>10009</v>
+        <v>10010</v>
       </c>
       <c r="C5014" s="1" t="s">
-        <v>9997</v>
+        <v>10006</v>
       </c>
     </row>
     <row r="5015" spans="1:3">
       <c r="A5015" s="1" t="s">
-        <v>10010</v>
+        <v>10011</v>
       </c>
       <c r="B5015" s="1" t="s">
-        <v>10011</v>
+        <v>10012</v>
       </c>
       <c r="C5015" s="1" t="s">
-        <v>9997</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="5016" spans="1:3">
       <c r="A5016" s="1" t="s">
-        <v>10012</v>
+        <v>10013</v>
       </c>
       <c r="B5016" s="1" t="s">
-        <v>10013</v>
+        <v>10014</v>
       </c>
       <c r="C5016" s="1" t="s">
-        <v>9997</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="5017" spans="1:3">
       <c r="A5017" s="1" t="s">
-        <v>10014</v>
+        <v>10015</v>
       </c>
       <c r="B5017" s="1" t="s">
-        <v>10015</v>
+        <v>10016</v>
       </c>
       <c r="C5017" s="1" t="s">
-        <v>10016</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="5018" spans="1:3">
@@ -85644,61 +85614,6 @@
         <v>10018</v>
       </c>
       <c r="C5018" s="1" t="s">
-        <v>10016</v>
-      </c>
-    </row>
-    <row r="5019" spans="1:3">
-      <c r="A5019" s="1" t="s">
-        <v>10019</v>
-      </c>
-      <c r="B5019" s="1" t="s">
-        <v>10020</v>
-      </c>
-      <c r="C5019" s="1" t="s">
-        <v>10016</v>
-      </c>
-    </row>
-    <row r="5020" spans="1:3">
-      <c r="A5020" s="1" t="s">
-        <v>10021</v>
-      </c>
-      <c r="B5020" s="1" t="s">
-        <v>10022</v>
-      </c>
-      <c r="C5020" s="1" t="s">
-        <v>9968</v>
-      </c>
-    </row>
-    <row r="5021" spans="1:3">
-      <c r="A5021" s="1" t="s">
-        <v>10023</v>
-      </c>
-      <c r="B5021" s="1" t="s">
-        <v>10024</v>
-      </c>
-      <c r="C5021" s="1" t="s">
-        <v>9968</v>
-      </c>
-    </row>
-    <row r="5022" spans="1:3">
-      <c r="A5022" s="1" t="s">
-        <v>10025</v>
-      </c>
-      <c r="B5022" s="1" t="s">
-        <v>10026</v>
-      </c>
-      <c r="C5022" s="1" t="s">
-        <v>9968</v>
-      </c>
-    </row>
-    <row r="5023" spans="1:3">
-      <c r="A5023" s="1" t="s">
-        <v>10027</v>
-      </c>
-      <c r="B5023" s="1" t="s">
-        <v>10028</v>
-      </c>
-      <c r="C5023" s="1" t="s">
         <v>9968</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove 8 Eudora Base Control Skin Perfection products from general DB
These products are IAF Make-only products and should only be used
for IAF penetration analysis, not for brand identification.

Removed SKUs: 84959, 84961, 84963, 84964, 84968, 84969, 84971, 84972

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/estoqueplanilha.xlsx
+++ b/data/estoqueplanilha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15051" uniqueCount="10019">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15027" uniqueCount="10003">
   <si>
     <t>SKU</t>
   </si>
@@ -29971,61 +29971,13 @@
     <t>GLAM GLOSS LAB TREAT AVELA SUTIL 5,4ml</t>
   </si>
   <si>
-    <t>84959</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 100F 30ml</t>
+    <t>53408</t>
+  </si>
+  <si>
+    <t>EUDORA GLAM BASE LIQUIDA SKIN CONTROL COR 55</t>
   </si>
   <si>
     <t>Eudora</t>
-  </si>
-  <si>
-    <t>84961</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 288Q 30ml</t>
-  </si>
-  <si>
-    <t>84963</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 170Q 30ml</t>
-  </si>
-  <si>
-    <t>84964</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 185F 30ml</t>
-  </si>
-  <si>
-    <t>84968</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 225Q 30ml</t>
-  </si>
-  <si>
-    <t>84969</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 235N 30ml</t>
-  </si>
-  <si>
-    <t>84971</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 260N 30ml</t>
-  </si>
-  <si>
-    <t>84972</t>
-  </si>
-  <si>
-    <t>EUDORA MAKE BASE LIQUIDA CONTROL SKIN PERFECTION 270Q 30ml</t>
-  </si>
-  <si>
-    <t>53408</t>
-  </si>
-  <si>
-    <t>EUDORA GLAM BASE LIQUIDA SKIN CONTROL COR 55</t>
   </si>
   <si>
     <t>55230</t>
@@ -30123,8 +30075,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5018" totalsRowShown="0">
-  <autoFilter ref="A1:C5018"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5010" totalsRowShown="0">
+  <autoFilter ref="A1:C5010"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SKU" dataDxfId="0"/>
     <tableColumn id="2" name="Nome" dataDxfId="0"/>
@@ -30419,7 +30371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5018"/>
+  <dimension ref="A1:C5010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -85460,160 +85412,72 @@
         <v>9989</v>
       </c>
       <c r="C5004" s="1" t="s">
-        <v>9987</v>
+        <v>9990</v>
       </c>
     </row>
     <row r="5005" spans="1:3">
       <c r="A5005" s="1" t="s">
+        <v>9991</v>
+      </c>
+      <c r="B5005" s="1" t="s">
+        <v>9992</v>
+      </c>
+      <c r="C5005" s="1" t="s">
         <v>9990</v>
-      </c>
-      <c r="B5005" s="1" t="s">
-        <v>9991</v>
-      </c>
-      <c r="C5005" s="1" t="s">
-        <v>9987</v>
       </c>
     </row>
     <row r="5006" spans="1:3">
       <c r="A5006" s="1" t="s">
-        <v>9992</v>
+        <v>9993</v>
       </c>
       <c r="B5006" s="1" t="s">
-        <v>9993</v>
+        <v>9994</v>
       </c>
       <c r="C5006" s="1" t="s">
-        <v>9987</v>
+        <v>9990</v>
       </c>
     </row>
     <row r="5007" spans="1:3">
       <c r="A5007" s="1" t="s">
-        <v>9994</v>
+        <v>9995</v>
       </c>
       <c r="B5007" s="1" t="s">
-        <v>9995</v>
+        <v>9996</v>
       </c>
       <c r="C5007" s="1" t="s">
-        <v>9987</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="5008" spans="1:3">
       <c r="A5008" s="1" t="s">
-        <v>9996</v>
+        <v>9997</v>
       </c>
       <c r="B5008" s="1" t="s">
-        <v>9997</v>
+        <v>9998</v>
       </c>
       <c r="C5008" s="1" t="s">
-        <v>9987</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="5009" spans="1:3">
       <c r="A5009" s="1" t="s">
-        <v>9998</v>
+        <v>9999</v>
       </c>
       <c r="B5009" s="1" t="s">
-        <v>9999</v>
+        <v>10000</v>
       </c>
       <c r="C5009" s="1" t="s">
-        <v>9987</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="5010" spans="1:3">
       <c r="A5010" s="1" t="s">
-        <v>10000</v>
+        <v>10001</v>
       </c>
       <c r="B5010" s="1" t="s">
-        <v>10001</v>
+        <v>10002</v>
       </c>
       <c r="C5010" s="1" t="s">
-        <v>9987</v>
-      </c>
-    </row>
-    <row r="5011" spans="1:3">
-      <c r="A5011" s="1" t="s">
-        <v>10002</v>
-      </c>
-      <c r="B5011" s="1" t="s">
-        <v>10003</v>
-      </c>
-      <c r="C5011" s="1" t="s">
-        <v>9987</v>
-      </c>
-    </row>
-    <row r="5012" spans="1:3">
-      <c r="A5012" s="1" t="s">
-        <v>10004</v>
-      </c>
-      <c r="B5012" s="1" t="s">
-        <v>10005</v>
-      </c>
-      <c r="C5012" s="1" t="s">
-        <v>10006</v>
-      </c>
-    </row>
-    <row r="5013" spans="1:3">
-      <c r="A5013" s="1" t="s">
-        <v>10007</v>
-      </c>
-      <c r="B5013" s="1" t="s">
-        <v>10008</v>
-      </c>
-      <c r="C5013" s="1" t="s">
-        <v>10006</v>
-      </c>
-    </row>
-    <row r="5014" spans="1:3">
-      <c r="A5014" s="1" t="s">
-        <v>10009</v>
-      </c>
-      <c r="B5014" s="1" t="s">
-        <v>10010</v>
-      </c>
-      <c r="C5014" s="1" t="s">
-        <v>10006</v>
-      </c>
-    </row>
-    <row r="5015" spans="1:3">
-      <c r="A5015" s="1" t="s">
-        <v>10011</v>
-      </c>
-      <c r="B5015" s="1" t="s">
-        <v>10012</v>
-      </c>
-      <c r="C5015" s="1" t="s">
-        <v>9968</v>
-      </c>
-    </row>
-    <row r="5016" spans="1:3">
-      <c r="A5016" s="1" t="s">
-        <v>10013</v>
-      </c>
-      <c r="B5016" s="1" t="s">
-        <v>10014</v>
-      </c>
-      <c r="C5016" s="1" t="s">
-        <v>9968</v>
-      </c>
-    </row>
-    <row r="5017" spans="1:3">
-      <c r="A5017" s="1" t="s">
-        <v>10015</v>
-      </c>
-      <c r="B5017" s="1" t="s">
-        <v>10016</v>
-      </c>
-      <c r="C5017" s="1" t="s">
-        <v>9968</v>
-      </c>
-    </row>
-    <row r="5018" spans="1:3">
-      <c r="A5018" s="1" t="s">
-        <v>10017</v>
-      </c>
-      <c r="B5018" s="1" t="s">
-        <v>10018</v>
-      </c>
-      <c r="C5018" s="1" t="s">
         <v>9968</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 31 missing SKUs to product database
Added flaconetes, kits, sachês, catálogos e guias:
- 15 O.U.I flaconetes/samples
- 5 Eudora products (including Siège Densihair kit)
- 9 oBoticário kits/sachês
- 1 AuAmigos flaconete
- 1 misc item

Total products: 5,038 (SQLite) / 5,040 (Excel)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/estoqueplanilha.xlsx
+++ b/data/estoqueplanilha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15027" uniqueCount="10003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15120" uniqueCount="10066">
   <si>
     <t>SKU</t>
   </si>
@@ -30023,6 +30023,195 @@
   </si>
   <si>
     <t>MAKE B BAT MATE AC/HIAL MALVA COOL 3,6g</t>
+  </si>
+  <si>
+    <t>48736</t>
+  </si>
+  <si>
+    <t>CBEM CR HID MAO NUVEM 50g V3</t>
+  </si>
+  <si>
+    <t>51788</t>
+  </si>
+  <si>
+    <t>CJ FLAC OUI EDP JD/GRASSE ROSE 3x1ml</t>
+  </si>
+  <si>
+    <t>58948</t>
+  </si>
+  <si>
+    <t>CJ FLAC BOLD INTENTION DES COL 3x1ml DOAÇÃO</t>
+  </si>
+  <si>
+    <t>58680</t>
+  </si>
+  <si>
+    <t>CJ FLAC OUI EDP LE FLANEUR 020 3x1ml</t>
+  </si>
+  <si>
+    <t>55468</t>
+  </si>
+  <si>
+    <t>SCH BOTIK SERUM FAC RESV/SILICIO 2ml</t>
+  </si>
+  <si>
+    <t>94332</t>
+  </si>
+  <si>
+    <t>CATALOGO OUI EDIC 01/2026 C1 A C4</t>
+  </si>
+  <si>
+    <t>83899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAC OUI EDP RIVIERE BLEUE 3x1ml </t>
+  </si>
+  <si>
+    <t>58392</t>
+  </si>
+  <si>
+    <t>CJ DEM BOTI D/COL FEM/MASC/INF V4 28x4ml</t>
+  </si>
+  <si>
+    <t>51506</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP ÉLÉGANCE ROYALE 115 VD 3x1ml</t>
+  </si>
+  <si>
+    <t>58115</t>
+  </si>
+  <si>
+    <t>SCH MEN SHAMP 2/1 ANTICASPA 3x7ml</t>
+  </si>
+  <si>
+    <t>59703</t>
+  </si>
+  <si>
+    <t>CJ SCH N/DERM ACT/PR SRUM/CR OLH/CR 3x2g</t>
+  </si>
+  <si>
+    <t>52006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAC OUI EDP SCAPIN 245 INTENSE 3X1ml </t>
+  </si>
+  <si>
+    <t>95337</t>
+  </si>
+  <si>
+    <t>GUIA EUDORA CICLO 04 2026 PRM</t>
+  </si>
+  <si>
+    <t>87562</t>
+  </si>
+  <si>
+    <t>CJ SCH SIAGE DENSI HAIR SH/COND/M 3x7ml</t>
+  </si>
+  <si>
+    <t>54123</t>
+  </si>
+  <si>
+    <t>EUDORA NEO DERMO PRO AGE CREME REPARADOR PESCOÇO E COLO 2ML DOÁVEL</t>
+  </si>
+  <si>
+    <t>52300</t>
+  </si>
+  <si>
+    <t>FLACONETE VOLPE NEXT DESODORANTE COLONIA, 3X1ML</t>
+  </si>
+  <si>
+    <t>83896</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP PARADIS ROUGE 3x1ml</t>
+  </si>
+  <si>
+    <t>86438</t>
+  </si>
+  <si>
+    <t>CJ SCH BOT SUN PROT INF FPS70 A/FL 4x5ml</t>
+  </si>
+  <si>
+    <t>82963</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP LEXPERIENCE 706 3x1ml</t>
+  </si>
+  <si>
+    <t>55847</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLACONETE EUDORA H DESODORANTE COLONIA FLOW 3X1ML	</t>
+  </si>
+  <si>
+    <t>88717</t>
+  </si>
+  <si>
+    <t>CJ FLAC MAGNIFIC DES COL PINK/PEON 3x1ml</t>
+  </si>
+  <si>
+    <t>87601</t>
+  </si>
+  <si>
+    <t>CJ SCH BOTIK SRUM F A/P AC/HIAL V2 5x2ml</t>
+  </si>
+  <si>
+    <t>88499</t>
+  </si>
+  <si>
+    <t>FLAC AU MIGOS PETS COL ADULT CHAMEGO 1ml</t>
+  </si>
+  <si>
+    <t>AuAmigos</t>
+  </si>
+  <si>
+    <t>58688</t>
+  </si>
+  <si>
+    <t>CJ FLAC OUI EDP MADEL 862 LA/PIST 3x1ml</t>
+  </si>
+  <si>
+    <t>82964</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP ICONIQUE 001 3x1ml</t>
+  </si>
+  <si>
+    <t>82962</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP LA VILLETTE 470 3x1ml</t>
+  </si>
+  <si>
+    <t>95806</t>
+  </si>
+  <si>
+    <t>GUIA EUDORA CICLO 05 2026 PRM</t>
+  </si>
+  <si>
+    <t>47612</t>
+  </si>
+  <si>
+    <t>CJ FLAC OUI EDP ELEGANCE ROYAL 115 3x1ml</t>
+  </si>
+  <si>
+    <t>82961</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP MADELEINE 862 3x1ml</t>
+  </si>
+  <si>
+    <t>82959</t>
+  </si>
+  <si>
+    <t>FLAC OUI EDP SCAPIN 245 3x1ml</t>
+  </si>
+  <si>
+    <t>46442</t>
+  </si>
+  <si>
+    <t>O BOTI FRASQ OFF WHITE VDA</t>
   </si>
 </sst>
 </file>
@@ -30075,8 +30264,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5010" totalsRowShown="0">
-  <autoFilter ref="A1:C5010"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C5041" totalsRowShown="0">
+  <autoFilter ref="A1:C5041"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SKU" dataDxfId="0"/>
     <tableColumn id="2" name="Nome" dataDxfId="0"/>
@@ -30371,7 +30560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5010"/>
+  <dimension ref="A1:C5041"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -85481,6 +85670,347 @@
         <v>9968</v>
       </c>
     </row>
+    <row r="5011" spans="1:3">
+      <c r="A5011" s="1" t="s">
+        <v>10003</v>
+      </c>
+      <c r="B5011" s="1" t="s">
+        <v>10004</v>
+      </c>
+      <c r="C5011" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5012" spans="1:3">
+      <c r="A5012" s="1" t="s">
+        <v>10005</v>
+      </c>
+      <c r="B5012" s="1" t="s">
+        <v>10006</v>
+      </c>
+      <c r="C5012" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5013" spans="1:3">
+      <c r="A5013" s="1" t="s">
+        <v>10007</v>
+      </c>
+      <c r="B5013" s="1" t="s">
+        <v>10008</v>
+      </c>
+      <c r="C5013" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5014" spans="1:3">
+      <c r="A5014" s="1" t="s">
+        <v>10009</v>
+      </c>
+      <c r="B5014" s="1" t="s">
+        <v>10010</v>
+      </c>
+      <c r="C5014" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5015" spans="1:3">
+      <c r="A5015" s="1" t="s">
+        <v>10011</v>
+      </c>
+      <c r="B5015" s="1" t="s">
+        <v>10012</v>
+      </c>
+      <c r="C5015" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5016" spans="1:3">
+      <c r="A5016" s="1" t="s">
+        <v>10013</v>
+      </c>
+      <c r="B5016" s="1" t="s">
+        <v>10014</v>
+      </c>
+      <c r="C5016" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5017" spans="1:3">
+      <c r="A5017" s="1" t="s">
+        <v>10015</v>
+      </c>
+      <c r="B5017" s="1" t="s">
+        <v>10016</v>
+      </c>
+      <c r="C5017" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5018" spans="1:3">
+      <c r="A5018" s="1" t="s">
+        <v>10017</v>
+      </c>
+      <c r="B5018" s="1" t="s">
+        <v>10018</v>
+      </c>
+      <c r="C5018" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5019" spans="1:3">
+      <c r="A5019" s="1" t="s">
+        <v>10019</v>
+      </c>
+      <c r="B5019" s="1" t="s">
+        <v>10020</v>
+      </c>
+      <c r="C5019" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5020" spans="1:3">
+      <c r="A5020" s="1" t="s">
+        <v>10021</v>
+      </c>
+      <c r="B5020" s="1" t="s">
+        <v>10022</v>
+      </c>
+      <c r="C5020" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5021" spans="1:3">
+      <c r="A5021" s="1" t="s">
+        <v>10023</v>
+      </c>
+      <c r="B5021" s="1" t="s">
+        <v>10024</v>
+      </c>
+      <c r="C5021" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5022" spans="1:3">
+      <c r="A5022" s="1" t="s">
+        <v>10025</v>
+      </c>
+      <c r="B5022" s="1" t="s">
+        <v>10026</v>
+      </c>
+      <c r="C5022" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5023" spans="1:3">
+      <c r="A5023" s="1" t="s">
+        <v>10027</v>
+      </c>
+      <c r="B5023" s="1" t="s">
+        <v>10028</v>
+      </c>
+      <c r="C5023" s="1" t="s">
+        <v>9987</v>
+      </c>
+    </row>
+    <row r="5024" spans="1:3">
+      <c r="A5024" s="1" t="s">
+        <v>10029</v>
+      </c>
+      <c r="B5024" s="1" t="s">
+        <v>10030</v>
+      </c>
+      <c r="C5024" s="1" t="s">
+        <v>9987</v>
+      </c>
+    </row>
+    <row r="5025" spans="1:3">
+      <c r="A5025" s="1" t="s">
+        <v>10031</v>
+      </c>
+      <c r="B5025" s="1" t="s">
+        <v>10032</v>
+      </c>
+      <c r="C5025" s="1" t="s">
+        <v>9987</v>
+      </c>
+    </row>
+    <row r="5026" spans="1:3">
+      <c r="A5026" s="1" t="s">
+        <v>10033</v>
+      </c>
+      <c r="B5026" s="1" t="s">
+        <v>10034</v>
+      </c>
+      <c r="C5026" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5027" spans="1:3">
+      <c r="A5027" s="1" t="s">
+        <v>10035</v>
+      </c>
+      <c r="B5027" s="1" t="s">
+        <v>10036</v>
+      </c>
+      <c r="C5027" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5028" spans="1:3">
+      <c r="A5028" s="1" t="s">
+        <v>10037</v>
+      </c>
+      <c r="B5028" s="1" t="s">
+        <v>10038</v>
+      </c>
+      <c r="C5028" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5029" spans="1:3">
+      <c r="A5029" s="1" t="s">
+        <v>10039</v>
+      </c>
+      <c r="B5029" s="1" t="s">
+        <v>10040</v>
+      </c>
+      <c r="C5029" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5030" spans="1:3">
+      <c r="A5030" s="1" t="s">
+        <v>10041</v>
+      </c>
+      <c r="B5030" s="1" t="s">
+        <v>10042</v>
+      </c>
+      <c r="C5030" s="1" t="s">
+        <v>9987</v>
+      </c>
+    </row>
+    <row r="5031" spans="1:3">
+      <c r="A5031" s="1" t="s">
+        <v>10043</v>
+      </c>
+      <c r="B5031" s="1" t="s">
+        <v>10044</v>
+      </c>
+      <c r="C5031" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5032" spans="1:3">
+      <c r="A5032" s="1" t="s">
+        <v>10045</v>
+      </c>
+      <c r="B5032" s="1" t="s">
+        <v>10046</v>
+      </c>
+      <c r="C5032" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="5033" spans="1:3">
+      <c r="A5033" s="1" t="s">
+        <v>10047</v>
+      </c>
+      <c r="B5033" s="1" t="s">
+        <v>10048</v>
+      </c>
+      <c r="C5033" s="1" t="s">
+        <v>10049</v>
+      </c>
+    </row>
+    <row r="5034" spans="1:3">
+      <c r="A5034" s="1" t="s">
+        <v>10050</v>
+      </c>
+      <c r="B5034" s="1" t="s">
+        <v>10051</v>
+      </c>
+      <c r="C5034" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5035" spans="1:3">
+      <c r="A5035" s="1" t="s">
+        <v>10052</v>
+      </c>
+      <c r="B5035" s="1" t="s">
+        <v>10053</v>
+      </c>
+      <c r="C5035" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5036" spans="1:3">
+      <c r="A5036" s="1" t="s">
+        <v>10054</v>
+      </c>
+      <c r="B5036" s="1" t="s">
+        <v>10055</v>
+      </c>
+      <c r="C5036" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5037" spans="1:3">
+      <c r="A5037" s="1" t="s">
+        <v>10056</v>
+      </c>
+      <c r="B5037" s="1" t="s">
+        <v>10057</v>
+      </c>
+      <c r="C5037" s="1" t="s">
+        <v>9987</v>
+      </c>
+    </row>
+    <row r="5038" spans="1:3">
+      <c r="A5038" s="1" t="s">
+        <v>10058</v>
+      </c>
+      <c r="B5038" s="1" t="s">
+        <v>10059</v>
+      </c>
+      <c r="C5038" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5039" spans="1:3">
+      <c r="A5039" s="1" t="s">
+        <v>10060</v>
+      </c>
+      <c r="B5039" s="1" t="s">
+        <v>10061</v>
+      </c>
+      <c r="C5039" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5040" spans="1:3">
+      <c r="A5040" s="1" t="s">
+        <v>10062</v>
+      </c>
+      <c r="B5040" s="1" t="s">
+        <v>10063</v>
+      </c>
+      <c r="C5040" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="5041" spans="1:3">
+      <c r="A5041" s="1" t="s">
+        <v>10064</v>
+      </c>
+      <c r="B5041" s="1" t="s">
+        <v>10065</v>
+      </c>
+      <c r="C5041" s="1" t="s">
+        <v>9968</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>